<commit_message>
fixed apfd and optimal
</commit_message>
<xml_diff>
--- a/resources/xlsx/BogoSort.xlsx
+++ b/resources/xlsx/BogoSort.xlsx
@@ -1,99 +1,84 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\github.com\PrioST\resources\xlsx\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0917B7F2-8510-410D-B30B-90D22C4CEC6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="600" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="BogoSortLongTC" sheetId="1" r:id="rId1"/>
-    <sheet name="BogoSortLongTC_PC" sheetId="2" r:id="rId2"/>
-    <sheet name="BogoSortLongTC_MACO" sheetId="3" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BogoSortLongTC" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BogoSortLongTC_PC" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BogoSortLongTC_MACO" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BogoSortShortTC_MACO" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BogoSortLongTC_Optimal" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="5">
-  <si>
-    <t>TC Order</t>
-  </si>
-  <si>
-    <t>APFD</t>
-  </si>
-  <si>
-    <t>['1', '2', '3', '4', '5', '6', '7']</t>
-  </si>
-  <si>
-    <t>['3', '5', '1', '6', '2', '4', '7']</t>
-  </si>
-  <si>
-    <t>['5', '3', '1', '6', '2', '4', '7']</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="9">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
+    </font>
+    <font>
       <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -191,44 +176,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -516,35 +520,97 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="3">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1">
+      <c r="A1" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>TC Order</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>APFD</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>0.35714285714285721</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>['1', '2', '3', '4', '5', '6', '7']</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.3571428571428572</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>['1', '2', '3', '4', '5', '6', '7']</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0.3571428571428572</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>['1', '2', '3', '4', '5', '6', '7']</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.3571428571428572</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>['1', '2', '3', '4', '5', '6', '7']</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.3571428571428572</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>['1', '2', '3', '4', '5', '6', '7']</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0.3571428571428572</v>
       </c>
     </row>
   </sheetData>
@@ -553,80 +619,122 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B1" s="1">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1">
+    <row r="1">
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>TC Order</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>APFD</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>['3', '5', '1', '6', '2', '4', '7']</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>['3', '5', '1', '6', '2', '4', '7']</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="C3">
-        <v>0.7142857142857143</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>0.7142857142857143</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>0.7142857142857143</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>['3', '5', '1', '6', '2', '4', '7']</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>0.7142857142857143</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>['3', '5', '1', '6', '2', '4', '7']</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>['3', '5', '1', '6', '2', '4', '7']</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>['3', '5', '1', '6', '2', '4', '7']</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0.7142857142857143</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -634,45 +742,242 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="3">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1">
+      <c r="A1" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>TC Order</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>APFD</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>['3', '5', '1', '6', '2', '4', '7']</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>['5', '3', '1', '6', '2', '4', '7']</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>['5', '3', '1', '6', '2', '4', '7']</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>['5', '3', '1']</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.3333333333333334</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>['5', '3', '1', '6', '2', '4', '7']</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>TC Order</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>APFD</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>0.7142857142857143</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>['5', '3', '1', '6', '2', '4', '7']</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>TC Order</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>APFD</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>['3', '5', '1']</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.3333333333333334</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>['3', '5', '1']</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0.3333333333333334</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>['3', '5', '1']</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.3333333333333334</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>['3', '5', '1', '2', '4', '6', '7']</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>['3', '5', '1', '2', '4', '6', '7']</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
         <v>0.7142857142857143</v>
       </c>
     </row>

</xml_diff>